<commit_message>
additional use rates, made weight consistently tons
</commit_message>
<xml_diff>
--- a/input/Modeparms(compare).xlsx
+++ b/input/Modeparms(compare).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fusio\Desktop\shoutlines_project\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pankaj\Desktop\shortlines_project\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950B25B9-7C51-4276-8FCE-DD52E7C87190}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" tabRatio="805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13290" tabRatio="805"/>
   </bookViews>
   <sheets>
     <sheet name="22-Mkt Share Frt-Trans time" sheetId="8" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <sheet name="Machinery(34)" sheetId="16" r:id="rId11"/>
     <sheet name="Mkt Share GC Models" sheetId="7" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="128">
   <si>
     <t>SCTG Description</t>
   </si>
@@ -382,9 +381,6 @@
     <t>bC</t>
   </si>
   <si>
-    <t>Table 22. Market-share two-digit SCTG models, transit times, and freight rates</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
@@ -433,7 +429,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="12">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -958,7 +954,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1128,9 +1124,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8934,7 +8927,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="112" workbookViewId="0" zoomToFit="1"/>
@@ -8945,7 +8938,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -8956,7 +8949,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -8967,7 +8960,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -8978,7 +8971,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -8989,7 +8982,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
@@ -9459,308 +9452,287 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
-        <v>113</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="36" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="46">
+        <v>21</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="46">
+        <v>5.0739999999999998</v>
+      </c>
+      <c r="D2" s="46">
+        <v>11.09</v>
+      </c>
+      <c r="E2" s="52">
+        <v>-3.6800000000000001E-3</v>
+      </c>
+      <c r="F2" s="46">
+        <v>-0.83</v>
+      </c>
+      <c r="G2" s="52">
+        <v>-3.9039999999999999E-3</v>
+      </c>
+      <c r="H2" s="46">
+        <v>-0.78</v>
+      </c>
+      <c r="I2" s="46">
+        <v>40</v>
+      </c>
+      <c r="J2" s="46">
+        <v>0.09</v>
+      </c>
+      <c r="K2" s="46">
+        <v>0.77</v>
+      </c>
+      <c r="L2" s="46">
+        <v>2.29</v>
+      </c>
+      <c r="M2" s="46">
+        <v>0.94</v>
+      </c>
+      <c r="N2" s="46">
         <v>1</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="N2" s="36" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="46">
-        <v>21</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="46">
-        <v>5.0739999999999998</v>
-      </c>
-      <c r="D3" s="46">
-        <v>11.09</v>
-      </c>
-      <c r="E3" s="52">
-        <v>-3.6800000000000001E-3</v>
-      </c>
-      <c r="F3" s="46">
-        <v>-0.83</v>
-      </c>
-      <c r="G3" s="52">
-        <v>-3.9039999999999999E-3</v>
-      </c>
-      <c r="H3" s="46">
-        <v>-0.78</v>
-      </c>
-      <c r="I3" s="46">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="36">
+        <v>6.3810000000000002</v>
+      </c>
+      <c r="D3" s="36">
+        <v>15.89</v>
+      </c>
+      <c r="E3" s="9">
+        <v>-5.8729999999999997E-3</v>
+      </c>
+      <c r="F3" s="36">
+        <v>-0.86</v>
+      </c>
+      <c r="G3" s="9">
+        <v>-4.9290000000000002E-3</v>
+      </c>
+      <c r="H3" s="36">
+        <v>-0.73</v>
+      </c>
+      <c r="I3" s="36">
         <v>40</v>
       </c>
-      <c r="J3" s="46">
-        <v>0.09</v>
-      </c>
-      <c r="K3" s="46">
-        <v>0.77</v>
-      </c>
-      <c r="L3" s="46">
-        <v>2.29</v>
-      </c>
-      <c r="M3" s="46">
-        <v>0.94</v>
-      </c>
-      <c r="N3" s="46">
+      <c r="J3" s="36">
+        <v>0.41</v>
+      </c>
+      <c r="K3" s="36">
+        <v>0.98</v>
+      </c>
+      <c r="L3" s="5">
+        <v>13</v>
+      </c>
+      <c r="M3" s="36">
+        <v>1.19</v>
+      </c>
+      <c r="N3" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="36">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="36">
-        <v>6.3810000000000002</v>
-      </c>
-      <c r="D4" s="36">
-        <v>15.89</v>
-      </c>
-      <c r="E4" s="9">
-        <v>-5.8729999999999997E-3</v>
-      </c>
-      <c r="F4" s="36">
-        <v>-0.86</v>
-      </c>
-      <c r="G4" s="9">
-        <v>-4.9290000000000002E-3</v>
-      </c>
-      <c r="H4" s="36">
-        <v>-0.73</v>
-      </c>
-      <c r="I4" s="36">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="46">
+        <v>30</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="46">
+        <v>5.6340000000000003</v>
+      </c>
+      <c r="D4" s="46">
+        <v>6.45</v>
+      </c>
+      <c r="E4" s="52">
+        <v>-2.872E-3</v>
+      </c>
+      <c r="F4" s="46">
+        <v>-0.94</v>
+      </c>
+      <c r="G4" s="52">
+        <v>-2.3839999999999998E-3</v>
+      </c>
+      <c r="H4" s="48">
+        <v>-0.7</v>
+      </c>
+      <c r="I4" s="46">
+        <v>35</v>
+      </c>
+      <c r="J4" s="46">
+        <v>0.27</v>
+      </c>
+      <c r="K4" s="48">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L4" s="46">
+        <v>7.98</v>
+      </c>
+      <c r="M4" s="48">
+        <v>1.2</v>
+      </c>
+      <c r="N4" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="46">
+        <v>37</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="36">
-        <v>0.41</v>
-      </c>
-      <c r="K4" s="36">
-        <v>0.98</v>
-      </c>
-      <c r="L4" s="5">
-        <v>13</v>
-      </c>
-      <c r="M4" s="36">
-        <v>1.19</v>
-      </c>
-      <c r="N4" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="46">
-        <v>30</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>65</v>
-      </c>
       <c r="C5" s="46">
-        <v>5.6340000000000003</v>
+        <v>3.532</v>
       </c>
       <c r="D5" s="46">
-        <v>6.45</v>
+        <v>11.14</v>
       </c>
       <c r="E5" s="52">
-        <v>-2.872E-3</v>
+        <v>-5.2240000000000003E-3</v>
       </c>
       <c r="F5" s="46">
-        <v>-0.94</v>
+        <v>-1.86</v>
       </c>
       <c r="G5" s="52">
-        <v>-2.3839999999999998E-3</v>
-      </c>
-      <c r="H5" s="48">
-        <v>-0.7</v>
+        <v>-5.9950000000000003E-3</v>
+      </c>
+      <c r="H5" s="46">
+        <v>-1.81</v>
       </c>
       <c r="I5" s="46">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="J5" s="46">
-        <v>0.27</v>
+        <v>0.05</v>
       </c>
       <c r="K5" s="48">
         <v>1.1000000000000001</v>
       </c>
       <c r="L5" s="46">
-        <v>7.98</v>
-      </c>
-      <c r="M5" s="48">
-        <v>1.2</v>
+        <v>2.04</v>
+      </c>
+      <c r="M5" s="46">
+        <v>0.87</v>
       </c>
       <c r="N5" s="46">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="46">
-        <v>37</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="46">
-        <v>3.532</v>
-      </c>
-      <c r="D6" s="46">
-        <v>11.14</v>
-      </c>
-      <c r="E6" s="52">
-        <v>-5.2240000000000003E-3</v>
-      </c>
-      <c r="F6" s="46">
-        <v>-1.86</v>
-      </c>
-      <c r="G6" s="52">
-        <v>-5.9950000000000003E-3</v>
-      </c>
-      <c r="H6" s="46">
-        <v>-1.81</v>
-      </c>
-      <c r="I6" s="46">
-        <v>40</v>
-      </c>
-      <c r="J6" s="46">
-        <v>0.05</v>
-      </c>
-      <c r="K6" s="48">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L6" s="46">
-        <v>2.04</v>
-      </c>
-      <c r="M6" s="46">
-        <v>0.87</v>
-      </c>
-      <c r="N6" s="46">
-        <v>1</v>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>41</v>
       </c>
@@ -9792,7 +9764,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>3</v>
       </c>
@@ -9827,7 +9799,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>5</v>
       </c>
@@ -9862,7 +9834,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>6</v>
       </c>
@@ -9897,7 +9869,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>7</v>
       </c>
@@ -9932,7 +9904,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>11</v>
       </c>
@@ -9964,7 +9936,7 @@
         <v>18.77</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>12</v>
       </c>
@@ -9996,7 +9968,7 @@
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>13</v>
       </c>
@@ -10028,7 +10000,7 @@
         <v>24.09</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>17</v>
       </c>
@@ -10060,7 +10032,7 @@
         <v>20.16</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>19</v>
       </c>
@@ -10092,7 +10064,7 @@
         <v>17.829999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>23</v>
       </c>
@@ -10124,7 +10096,7 @@
         <v>15.51</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>24</v>
       </c>
@@ -10156,7 +10128,7 @@
         <v>24.97</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>25</v>
       </c>
@@ -10188,7 +10160,7 @@
         <v>18.850000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>26</v>
       </c>
@@ -10220,13 +10192,13 @@
         <v>43.9</v>
       </c>
       <c r="L14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>27</v>
       </c>
@@ -10258,10 +10230,10 @@
         <v>51.99</v>
       </c>
       <c r="N15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>28</v>
       </c>
@@ -10293,10 +10265,10 @@
         <v>61.15</v>
       </c>
       <c r="N16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>29</v>
       </c>
@@ -10328,10 +10300,10 @@
         <v>17.559999999999999</v>
       </c>
       <c r="N17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="46">
         <v>30</v>
       </c>
@@ -10363,10 +10335,10 @@
         <v>9.5399999999999991</v>
       </c>
       <c r="N18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>31</v>
       </c>
@@ -10398,7 +10370,7 @@
         <v>10.09</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>32</v>
       </c>
@@ -10430,7 +10402,7 @@
         <v>13.77</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>33</v>
       </c>
@@ -10462,7 +10434,7 @@
         <v>23.91</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>34</v>
       </c>
@@ -10494,7 +10466,7 @@
         <v>13.39</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>35</v>
       </c>
@@ -10526,7 +10498,7 @@
         <v>7.18</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>39</v>
       </c>
@@ -10558,7 +10530,7 @@
         <v>51.37</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>43</v>
       </c>
@@ -10590,7 +10562,7 @@
         <v>38.119999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="17" t="s">
         <v>67</v>
@@ -10604,7 +10576,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>2</v>
       </c>
@@ -10636,7 +10608,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>4</v>
       </c>
@@ -10668,7 +10640,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>8</v>
       </c>
@@ -10700,7 +10672,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>10</v>
       </c>
@@ -10732,7 +10704,7 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>18</v>
       </c>
@@ -10764,7 +10736,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>38</v>
       </c>
@@ -10796,7 +10768,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>40</v>
       </c>
@@ -10828,7 +10800,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>41</v>
       </c>
@@ -10866,43 +10838,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU74"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G1" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" customWidth="1"/>
-    <col min="19" max="20" width="14.6640625" customWidth="1"/>
-    <col min="21" max="21" width="9.5546875" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" customWidth="1"/>
-    <col min="23" max="24" width="9.6640625" customWidth="1"/>
-    <col min="25" max="26" width="9.5546875" customWidth="1"/>
-    <col min="27" max="27" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.88671875" customWidth="1"/>
-    <col min="30" max="30" width="10.109375" customWidth="1"/>
-    <col min="32" max="32" width="10.33203125" customWidth="1"/>
-    <col min="33" max="33" width="10.44140625" customWidth="1"/>
-    <col min="34" max="34" width="12.44140625" customWidth="1"/>
-    <col min="35" max="35" width="10.6640625" customWidth="1"/>
-    <col min="36" max="36" width="11.88671875" customWidth="1"/>
-    <col min="37" max="37" width="11.33203125" customWidth="1"/>
-    <col min="39" max="40" width="12.6640625" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="20" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" customWidth="1"/>
+    <col min="23" max="24" width="9.7109375" customWidth="1"/>
+    <col min="25" max="26" width="9.5703125" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.85546875" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" customWidth="1"/>
+    <col min="32" max="32" width="10.28515625" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" customWidth="1"/>
+    <col min="34" max="34" width="12.42578125" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" customWidth="1"/>
+    <col min="37" max="37" width="11.28515625" customWidth="1"/>
+    <col min="39" max="40" width="12.7109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
     <col min="43" max="43" width="11" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" customWidth="1"/>
+    <col min="44" max="44" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>41</v>
       </c>
@@ -10925,7 +10897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" t="s">
         <v>36</v>
@@ -10940,7 +10912,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
       <c r="AC2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE2">
         <v>1000</v>
@@ -10949,7 +10921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="46">
         <v>2</v>
       </c>
@@ -10973,7 +10945,7 @@
       </c>
       <c r="H3" s="51"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="46">
         <v>3</v>
       </c>
@@ -10997,7 +10969,7 @@
       </c>
       <c r="H4" s="51"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>4</v>
       </c>
@@ -11021,7 +10993,7 @@
       </c>
       <c r="H5" s="51"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="46">
         <v>5</v>
       </c>
@@ -11054,7 +11026,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="46">
         <v>6</v>
       </c>
@@ -11077,26 +11049,26 @@
         <v>1</v>
       </c>
       <c r="H7" s="51"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74" t="s">
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74" t="s">
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R7" s="74"/>
-      <c r="S7" s="74" t="s">
+      <c r="R7" s="73"/>
+      <c r="S7" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T7" s="74"/>
+      <c r="T7" s="73"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="46">
         <v>7</v>
       </c>
@@ -11126,25 +11098,25 @@
         <v>59</v>
       </c>
       <c r="L8" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="70" t="s">
         <v>116</v>
-      </c>
-      <c r="M8" s="70" t="s">
-        <v>117</v>
       </c>
       <c r="N8" s="70" t="s">
         <v>58</v>
       </c>
       <c r="O8" s="70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P8" s="70" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q8" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R8" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S8" s="13" t="s">
         <v>51</v>
@@ -11221,7 +11193,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="42">
         <v>8</v>
       </c>
@@ -11376,7 +11348,7 @@
         <v>1.3831195702507971E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="42">
         <v>9</v>
       </c>
@@ -11531,7 +11503,7 @@
         <v>2.5989242033571456E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>11</v>
       </c>
@@ -11686,7 +11658,7 @@
         <v>1.6538427162146222E-13</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>12</v>
       </c>
@@ -11841,7 +11813,7 @@
         <v>3.6139020584157028E-27</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>13</v>
       </c>
@@ -11996,12 +11968,12 @@
         <v>1.7256023576958091E-54</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>15</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="46">
@@ -12147,7 +12119,7 @@
         <v>1.8785976149456325E-136</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>17</v>
       </c>
@@ -12198,7 +12170,7 @@
         <v>4.6628935595663493E-273</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="42">
         <v>18</v>
       </c>
@@ -12258,7 +12230,7 @@
         <v>0.10628227817886907</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="46">
         <v>19</v>
       </c>
@@ -12279,24 +12251,24 @@
         <v>6</v>
       </c>
       <c r="H17" s="51"/>
-      <c r="K17" s="74" t="s">
+      <c r="K17" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74" t="s">
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74" t="s">
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R17" s="74"/>
-      <c r="S17" s="74" t="s">
+      <c r="R17" s="73"/>
+      <c r="S17" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T17" s="74"/>
+      <c r="T17" s="73"/>
       <c r="AE17">
         <v>50</v>
       </c>
@@ -12346,7 +12318,7 @@
         <v>1.5366486627634539E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="46">
         <v>20</v>
       </c>
@@ -12376,25 +12348,25 @@
         <v>59</v>
       </c>
       <c r="L18" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="M18" s="37" t="s">
         <v>116</v>
-      </c>
-      <c r="M18" s="37" t="s">
-        <v>117</v>
       </c>
       <c r="N18" s="37" t="s">
         <v>58</v>
       </c>
       <c r="O18" s="37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P18" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q18" s="40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R18" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S18" s="37" t="s">
         <v>51</v>
@@ -12476,7 +12448,7 @@
         <v>3.3172930395968849E-13</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="46">
         <v>22</v>
       </c>
@@ -12625,7 +12597,7 @@
         <v>1.1958811703014522E-27</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="46">
         <v>23</v>
       </c>
@@ -12774,7 +12746,7 @@
         <v>1.5541624377855266E-56</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="46">
         <v>24</v>
       </c>
@@ -12923,7 +12895,7 @@
         <v>3.4113128501218371E-143</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="46">
         <v>25</v>
       </c>
@@ -13072,7 +13044,7 @@
         <v>1.2646299218358749E-287</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="46">
         <v>26</v>
       </c>
@@ -13221,7 +13193,7 @@
         <v>0.91490639919487449</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="46">
         <v>27</v>
       </c>
@@ -13370,7 +13342,7 @@
         <v>0.17395391674558203</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="46">
         <v>28</v>
       </c>
@@ -13421,7 +13393,7 @@
         <v>1.5822669753640921E-6</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="42">
         <v>29</v>
       </c>
@@ -13502,7 +13474,7 @@
         <v>4.5606979453117276E-15</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="46">
         <v>31</v>
       </c>
@@ -13525,24 +13497,24 @@
         <v>2</v>
       </c>
       <c r="H27" s="51"/>
-      <c r="K27" s="74" t="s">
+      <c r="K27" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="74"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="74" t="s">
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O27" s="74"/>
-      <c r="P27" s="74"/>
-      <c r="Q27" s="74" t="s">
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R27" s="74"/>
-      <c r="S27" s="74" t="s">
+      <c r="R27" s="73"/>
+      <c r="S27" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T27" s="74"/>
+      <c r="T27" s="73"/>
       <c r="AC27">
         <v>13</v>
       </c>
@@ -13598,7 +13570,7 @@
         <v>3.7890734843686439E-32</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="46">
         <v>32</v>
       </c>
@@ -13628,25 +13600,25 @@
         <v>59</v>
       </c>
       <c r="L28" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="M28" s="37" t="s">
         <v>116</v>
-      </c>
-      <c r="M28" s="37" t="s">
-        <v>117</v>
       </c>
       <c r="N28" s="37" t="s">
         <v>58</v>
       </c>
       <c r="O28" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="P28" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q28" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="P28" s="37" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q28" s="37" t="s">
+      <c r="R28" s="37" t="s">
         <v>120</v>
-      </c>
-      <c r="R28" s="37" t="s">
-        <v>121</v>
       </c>
       <c r="S28" s="37" t="s">
         <v>51</v>
@@ -13728,7 +13700,7 @@
         <v>2.1728922059249977E-83</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="46">
         <v>33</v>
       </c>
@@ -13876,7 +13848,7 @@
         <v>8.6009569201278596E-169</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="46">
         <v>34</v>
       </c>
@@ -14024,7 +13996,7 @@
         <v>2.7901216680752679E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="46">
         <v>35</v>
       </c>
@@ -14172,7 +14144,7 @@
         <v>7.9354713142512444E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="46">
         <v>36</v>
       </c>
@@ -14320,7 +14292,7 @@
         <v>1.8104334832470038E-17</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="46">
         <v>38</v>
       </c>
@@ -14468,7 +14440,7 @@
         <v>3.3225006698477309E-35</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="42">
         <v>39</v>
       </c>
@@ -14589,7 +14561,7 @@
         <v>1.1189999967546572E-70</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="46">
         <v>40</v>
       </c>
@@ -14661,7 +14633,7 @@
         <v>4.2748916287267471E-177</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="46">
         <v>41</v>
       </c>
@@ -14748,7 +14720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" s="46">
         <v>43</v>
       </c>
@@ -14771,24 +14743,24 @@
         <v>1</v>
       </c>
       <c r="H37" s="51"/>
-      <c r="K37" s="74" t="s">
+      <c r="K37" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74" t="s">
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74" t="s">
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74" t="s">
+      <c r="R37" s="73"/>
+      <c r="S37" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T37" s="74"/>
+      <c r="T37" s="73"/>
       <c r="AC37">
         <v>20</v>
       </c>
@@ -14844,7 +14816,7 @@
         <v>1.5041681989268023E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J38" s="53" t="s">
         <v>46</v>
       </c>
@@ -14852,25 +14824,25 @@
         <v>59</v>
       </c>
       <c r="L38" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M38" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M38" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N38" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O38" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P38" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q38" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P38" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q38" s="53" t="s">
+      <c r="R38" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R38" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S38" s="53" t="s">
         <v>51</v>
@@ -14952,7 +14924,7 @@
         <v>4.202421271898308E-8</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
       <c r="I39" s="53">
         <f>I$9</f>
@@ -15080,9 +15052,9 @@
         <v>9.1232164449243225E-22</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I40" s="53">
         <f>I$10</f>
@@ -15210,9 +15182,9 @@
         <v>1.5413287121845216E-44</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I41" s="53">
         <f>I$11</f>
@@ -15340,9 +15312,9 @@
         <v>4.3993635163369094E-90</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I42" s="53">
         <f>I$12</f>
@@ -15470,9 +15442,9 @@
         <v>1.0229951854984894E-226</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I43" s="53">
         <f>I$13</f>
@@ -15573,9 +15545,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I44" s="53">
         <f>I$14</f>
@@ -15697,7 +15669,7 @@
         <v>0.94750738686686531</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
       <c r="AC45">
         <v>26</v>
       </c>
@@ -15753,7 +15725,7 @@
         <v>0.55436536265605862</v>
       </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J46" t="s">
         <v>55</v>
       </c>
@@ -15818,25 +15790,25 @@
         <v>4.0704136404339772E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="K47" s="74" t="s">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="K47" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L47" s="74"/>
-      <c r="M47" s="74"/>
-      <c r="N47" s="74" t="s">
+      <c r="L47" s="73"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O47" s="74"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="74" t="s">
+      <c r="O47" s="73"/>
+      <c r="P47" s="73"/>
+      <c r="Q47" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R47" s="74"/>
-      <c r="S47" s="74" t="s">
+      <c r="R47" s="73"/>
+      <c r="S47" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T47" s="74"/>
+      <c r="T47" s="73"/>
       <c r="AC47">
         <v>26</v>
       </c>
@@ -15892,7 +15864,7 @@
         <v>6.3310980295955704E-10</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J48" s="53" t="s">
         <v>46</v>
       </c>
@@ -15900,25 +15872,25 @@
         <v>59</v>
       </c>
       <c r="L48" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M48" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M48" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N48" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O48" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P48" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q48" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P48" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q48" s="53" t="s">
+      <c r="R48" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R48" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S48" s="53" t="s">
         <v>51</v>
@@ -16000,7 +15972,7 @@
         <v>1.530405090309095E-21</v>
       </c>
     </row>
-    <row r="49" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I49" s="53">
         <f>I$9</f>
         <v>34</v>
@@ -16127,7 +16099,7 @@
         <v>2.1616654983927735E-56</v>
       </c>
     </row>
-    <row r="50" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I50" s="53">
         <f>I$10</f>
         <v>27</v>
@@ -16254,7 +16226,7 @@
         <v>1.7841251147541342E-114</v>
       </c>
     </row>
-    <row r="51" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I51" s="53">
         <f>I$11</f>
         <v>26</v>
@@ -16359,7 +16331,7 @@
       <c r="AQ51" s="6"/>
       <c r="AR51" s="6"/>
     </row>
-    <row r="52" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="52" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I52" s="53">
         <f>I$12</f>
         <v>20</v>
@@ -16437,7 +16409,7 @@
       <c r="AQ52" s="6"/>
       <c r="AR52" s="6"/>
     </row>
-    <row r="53" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="53" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I53" s="53">
         <f>I$13</f>
         <v>2</v>
@@ -16536,7 +16508,7 @@
       <c r="AQ53" s="6"/>
       <c r="AR53" s="6"/>
     </row>
-    <row r="54" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="54" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I54" s="53">
         <f>I$14</f>
         <v>13</v>
@@ -16641,7 +16613,7 @@
       <c r="AQ54" s="6"/>
       <c r="AR54" s="6"/>
     </row>
-    <row r="55" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="55" spans="9:47" x14ac:dyDescent="0.25">
       <c r="AC55">
         <v>27</v>
       </c>
@@ -16675,7 +16647,7 @@
       <c r="AQ55" s="6"/>
       <c r="AR55" s="6"/>
     </row>
-    <row r="56" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="56" spans="9:47" x14ac:dyDescent="0.25">
       <c r="J56" t="s">
         <v>55</v>
       </c>
@@ -16718,7 +16690,7 @@
       <c r="AQ56" s="6"/>
       <c r="AR56" s="6"/>
     </row>
-    <row r="57" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="57" spans="9:47" x14ac:dyDescent="0.25">
       <c r="K57" s="53" t="s">
         <v>51</v>
       </c>
@@ -16770,7 +16742,7 @@
       <c r="AQ57" s="6"/>
       <c r="AR57" s="6"/>
     </row>
-    <row r="58" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="58" spans="9:47" x14ac:dyDescent="0.25">
       <c r="J58" s="53" t="s">
         <v>46</v>
       </c>
@@ -16778,25 +16750,25 @@
         <v>59</v>
       </c>
       <c r="L58" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M58" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M58" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N58" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O58" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P58" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q58" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P58" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q58" s="53" t="s">
+      <c r="R58" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R58" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S58" s="53" t="s">
         <v>51</v>
@@ -16855,7 +16827,7 @@
       <c r="AQ58" s="6"/>
       <c r="AR58" s="6"/>
     </row>
-    <row r="59" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="59" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I59" s="53">
         <f>I$9</f>
         <v>34</v>
@@ -16959,7 +16931,7 @@
       <c r="AQ59" s="6"/>
       <c r="AR59" s="6"/>
     </row>
-    <row r="60" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="60" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I60" s="53">
         <f>I$10</f>
         <v>27</v>
@@ -17058,7 +17030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="61" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I61" s="53">
         <f>I$11</f>
         <v>26</v>
@@ -17130,7 +17102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="62" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I62" s="53">
         <f>I$12</f>
         <v>20</v>
@@ -17223,7 +17195,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="63" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="63" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I63" s="53">
         <f>I$13</f>
         <v>2</v>
@@ -17322,7 +17294,7 @@
         <v>0.94750738686686531</v>
       </c>
     </row>
-    <row r="64" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="64" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I64" s="37">
         <f>I$14</f>
         <v>13</v>
@@ -17421,7 +17393,7 @@
         <v>0.55436536265605862</v>
       </c>
     </row>
-    <row r="65" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="9:37" x14ac:dyDescent="0.25">
       <c r="AC65">
         <v>34</v>
       </c>
@@ -17450,7 +17422,7 @@
         <v>4.0704136404339772E-4</v>
       </c>
     </row>
-    <row r="66" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="9:37" x14ac:dyDescent="0.25">
       <c r="J66" t="s">
         <v>55</v>
       </c>
@@ -17488,7 +17460,7 @@
         <v>6.3310980295955704E-10</v>
       </c>
     </row>
-    <row r="67" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="9:37" x14ac:dyDescent="0.25">
       <c r="K67" s="53" t="s">
         <v>51</v>
       </c>
@@ -17535,7 +17507,7 @@
         <v>1.530405090309095E-21</v>
       </c>
     </row>
-    <row r="68" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="9:37" x14ac:dyDescent="0.25">
       <c r="J68" s="53" t="s">
         <v>46</v>
       </c>
@@ -17543,25 +17515,25 @@
         <v>59</v>
       </c>
       <c r="L68" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M68" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M68" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N68" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O68" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P68" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q68" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P68" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q68" s="53" t="s">
+      <c r="R68" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R68" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S68" s="53" t="s">
         <v>51</v>
@@ -17615,7 +17587,7 @@
         <v>2.1616654983927735E-56</v>
       </c>
     </row>
-    <row r="69" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I69" s="53">
         <f>I$9</f>
         <v>34</v>
@@ -17714,7 +17686,7 @@
         <v>1.7841251147541342E-114</v>
       </c>
     </row>
-    <row r="70" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I70" s="53">
         <f>I$10</f>
         <v>27</v>
@@ -17787,7 +17759,7 @@
       </c>
       <c r="AC70" s="15"/>
     </row>
-    <row r="71" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I71" s="53">
         <f>I$11</f>
         <v>26</v>
@@ -17859,7 +17831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I72" s="53">
         <f>I$12</f>
         <v>20</v>
@@ -17932,7 +17904,7 @@
       </c>
       <c r="AC72" s="15"/>
     </row>
-    <row r="73" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I73" s="53">
         <f>I$13</f>
         <v>2</v>
@@ -18005,7 +17977,7 @@
       </c>
       <c r="AC73" s="15"/>
     </row>
-    <row r="74" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I74" s="53">
         <f>I$14</f>
         <v>13</v>
@@ -18078,19 +18050,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AM9:AU50">
+  <sortState ref="AM9:AU50">
     <sortCondition ref="AM9:AM50"/>
     <sortCondition ref="AN9:AN50"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="K47:M47"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="S47:T47"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="S27:T27"/>
@@ -18103,6 +18067,14 @@
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="N17:P17"/>
     <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="K47:M47"/>
+    <mergeCell ref="N47:P47"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="S47:T47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18110,43 +18082,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU74"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="25.33203125" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" customWidth="1"/>
-    <col min="19" max="20" width="14.6640625" customWidth="1"/>
-    <col min="21" max="21" width="9.5546875" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" customWidth="1"/>
-    <col min="23" max="24" width="9.6640625" customWidth="1"/>
-    <col min="25" max="26" width="9.5546875" customWidth="1"/>
-    <col min="27" max="27" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.88671875" customWidth="1"/>
-    <col min="30" max="30" width="10.109375" customWidth="1"/>
-    <col min="32" max="32" width="10.33203125" customWidth="1"/>
-    <col min="33" max="33" width="10.44140625" customWidth="1"/>
-    <col min="34" max="34" width="12.44140625" customWidth="1"/>
-    <col min="35" max="35" width="10.6640625" customWidth="1"/>
-    <col min="36" max="36" width="11.88671875" customWidth="1"/>
-    <col min="37" max="37" width="11.33203125" customWidth="1"/>
-    <col min="39" max="40" width="12.6640625" customWidth="1"/>
-    <col min="42" max="42" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="19" max="20" width="14.7109375" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" customWidth="1"/>
+    <col min="23" max="24" width="9.7109375" customWidth="1"/>
+    <col min="25" max="26" width="9.5703125" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.85546875" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" customWidth="1"/>
+    <col min="32" max="32" width="10.28515625" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" customWidth="1"/>
+    <col min="34" max="34" width="12.42578125" customWidth="1"/>
+    <col min="35" max="35" width="10.7109375" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" customWidth="1"/>
+    <col min="37" max="37" width="11.28515625" customWidth="1"/>
+    <col min="39" max="40" width="12.7109375" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" customWidth="1"/>
     <col min="43" max="43" width="11" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" customWidth="1"/>
+    <col min="44" max="44" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="56" t="s">
         <v>41</v>
       </c>
@@ -18169,7 +18141,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="56"/>
       <c r="B2" s="57" t="s">
         <v>36</v>
@@ -18184,7 +18156,7 @@
       <c r="F2" s="56"/>
       <c r="G2" s="56"/>
       <c r="AC2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE2">
         <v>500</v>
@@ -18193,7 +18165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="60">
         <v>2</v>
       </c>
@@ -18217,7 +18189,7 @@
       </c>
       <c r="H3" s="51"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" s="60">
         <v>3</v>
       </c>
@@ -18241,7 +18213,7 @@
       </c>
       <c r="H4" s="51"/>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" s="60">
         <v>4</v>
       </c>
@@ -18265,7 +18237,7 @@
       </c>
       <c r="H5" s="51"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" s="60">
         <v>5</v>
       </c>
@@ -18298,7 +18270,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" s="60">
         <v>6</v>
       </c>
@@ -18321,26 +18293,26 @@
         <v>1</v>
       </c>
       <c r="H7" s="51"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74" t="s">
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
+      <c r="N7" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="75" t="s">
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="R7" s="75"/>
-      <c r="S7" s="74" t="s">
+      <c r="R7" s="74"/>
+      <c r="S7" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T7" s="74"/>
+      <c r="T7" s="73"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="60">
         <v>7</v>
       </c>
@@ -18370,25 +18342,25 @@
         <v>59</v>
       </c>
       <c r="L8" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M8" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N8" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O8" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P8" s="53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q8" s="56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R8" s="56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S8" s="53" t="s">
         <v>51</v>
@@ -18465,7 +18437,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="64">
         <v>8</v>
       </c>
@@ -18620,7 +18592,7 @@
         <v>6.7710698398440405E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" s="64">
         <v>9</v>
       </c>
@@ -18775,7 +18747,7 @@
         <v>6.9646384863490294E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" s="60">
         <v>11</v>
       </c>
@@ -18930,7 +18902,7 @@
         <v>6.1586402805559476E-10</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" s="60">
         <v>12</v>
       </c>
@@ -19085,7 +19057,7 @@
         <v>5.0113835779795696E-20</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" s="60">
         <v>13</v>
       </c>
@@ -19240,12 +19212,12 @@
         <v>3.3182053531006388E-40</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" s="60">
         <v>15</v>
       </c>
       <c r="B14" s="61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="61"/>
       <c r="D14" s="60">
@@ -19391,7 +19363,7 @@
         <v>9.6325240492643967E-101</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" s="60">
         <v>17</v>
       </c>
@@ -19442,7 +19414,7 @@
         <v>1.2259370561777919E-201</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" s="64">
         <v>18</v>
       </c>
@@ -19502,7 +19474,7 @@
         <v>0.44587848067430369</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A17" s="60">
         <v>19</v>
       </c>
@@ -19523,24 +19495,24 @@
         <v>6</v>
       </c>
       <c r="H17" s="51"/>
-      <c r="K17" s="74" t="s">
+      <c r="K17" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74" t="s">
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74" t="s">
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
+      <c r="Q17" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R17" s="74"/>
-      <c r="S17" s="74" t="s">
+      <c r="R17" s="73"/>
+      <c r="S17" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T17" s="74"/>
+      <c r="T17" s="73"/>
       <c r="AE17">
         <v>50</v>
       </c>
@@ -19590,7 +19562,7 @@
         <v>6.9871203978715841E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="60">
         <v>20</v>
       </c>
@@ -19620,25 +19592,25 @@
         <v>59</v>
       </c>
       <c r="L18" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M18" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M18" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N18" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O18" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P18" s="53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q18" s="53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R18" s="53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S18" s="53" t="s">
         <v>51</v>
@@ -19720,7 +19692,7 @@
         <v>4.7047753468511494E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="60">
         <v>22</v>
       </c>
@@ -19869,7 +19841,7 @@
         <v>2.4054599933732609E-19</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A20" s="60">
         <v>23</v>
       </c>
@@ -20018,7 +19990,7 @@
         <v>6.2880593103970914E-40</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A21" s="60">
         <v>24</v>
       </c>
@@ -20167,7 +20139,7 @@
         <v>1.1232388153158255E-101</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="60">
         <v>25</v>
       </c>
@@ -20316,7 +20288,7 @@
         <v>1.3710855645636452E-204</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A23" s="60">
         <v>26</v>
       </c>
@@ -20465,7 +20437,7 @@
         <v>0.97296647562204686</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A24" s="60">
         <v>27</v>
       </c>
@@ -20614,7 +20586,7 @@
         <v>0.70235631744962801</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="60">
         <v>28</v>
       </c>
@@ -20665,7 +20637,7 @@
         <v>6.6461316284611039E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A26" s="64">
         <v>29</v>
       </c>
@@ -20746,7 +20718,7 @@
         <v>8.0572298326311081E-10</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A27" s="60">
         <v>31</v>
       </c>
@@ -20769,24 +20741,24 @@
         <v>2</v>
       </c>
       <c r="H27" s="51"/>
-      <c r="K27" s="74" t="s">
+      <c r="K27" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="74"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="74" t="s">
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O27" s="74"/>
-      <c r="P27" s="74"/>
-      <c r="Q27" s="74" t="s">
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R27" s="74"/>
-      <c r="S27" s="74" t="s">
+      <c r="R27" s="73"/>
+      <c r="S27" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T27" s="74"/>
+      <c r="T27" s="73"/>
       <c r="AC27">
         <v>13</v>
       </c>
@@ -20842,7 +20814,7 @@
         <v>1.1826109966251357E-21</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="60">
         <v>32</v>
       </c>
@@ -20872,25 +20844,25 @@
         <v>59</v>
       </c>
       <c r="L28" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M28" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M28" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N28" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O28" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P28" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q28" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P28" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q28" s="53" t="s">
+      <c r="R28" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R28" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S28" s="53" t="s">
         <v>51</v>
@@ -20972,7 +20944,7 @@
         <v>3.7394729389817085E-57</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A29" s="60">
         <v>33</v>
       </c>
@@ -21120,7 +21092,7 @@
         <v>2.54736511867457E-116</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="60">
         <v>34</v>
       </c>
@@ -21268,7 +21240,7 @@
         <v>2.9634390362074756E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="60">
         <v>35</v>
       </c>
@@ -21416,7 +21388,7 @@
         <v>9.4532267657788032E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A32" s="60">
         <v>36</v>
       </c>
@@ -21564,7 +21536,7 @@
         <v>2.8048053570399042E-12</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" s="60">
         <v>38</v>
       </c>
@@ -21712,7 +21684,7 @@
         <v>7.974535346999028E-25</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" s="64">
         <v>39</v>
       </c>
@@ -21833,7 +21805,7 @@
         <v>6.446302860534334E-50</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="60">
         <v>40</v>
       </c>
@@ -21905,7 +21877,7 @@
         <v>3.4050748317249211E-125</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" s="60">
         <v>41</v>
       </c>
@@ -21992,7 +21964,7 @@
         <v>1.1753122215225618E-250</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" s="60">
         <v>43</v>
       </c>
@@ -22015,24 +21987,24 @@
         <v>1</v>
       </c>
       <c r="H37" s="51"/>
-      <c r="K37" s="74" t="s">
+      <c r="K37" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74" t="s">
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74" t="s">
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74" t="s">
+      <c r="R37" s="73"/>
+      <c r="S37" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T37" s="74"/>
+      <c r="T37" s="73"/>
       <c r="AC37">
         <v>20</v>
       </c>
@@ -22088,7 +22060,7 @@
         <v>3.3553350772809347E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J38" s="53" t="s">
         <v>46</v>
       </c>
@@ -22096,25 +22068,25 @@
         <v>59</v>
       </c>
       <c r="L38" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M38" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M38" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N38" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O38" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P38" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q38" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P38" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q38" s="53" t="s">
+      <c r="R38" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R38" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S38" s="53" t="s">
         <v>51</v>
@@ -22196,7 +22168,7 @@
         <v>2.2320588590073856E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
       <c r="I39" s="53">
         <f>I$9</f>
@@ -22324,9 +22296,9 @@
         <v>5.93181105124839E-15</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I40" s="53">
         <f>I$10</f>
@@ -22454,9 +22426,9 @@
         <v>6.5158927793522681E-31</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I41" s="53">
         <f>I$11</f>
@@ -22584,9 +22556,9 @@
         <v>7.8622558119722086E-63</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I42" s="53">
         <f>I$12</f>
@@ -22714,9 +22686,9 @@
         <v>1.3812328323043235E-158</v>
       </c>
     </row>
-    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I43" s="53">
         <f>I$13</f>
@@ -22817,9 +22789,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I44" s="53">
         <f>I$14</f>
@@ -22941,7 +22913,7 @@
         <v>0.98867289643278788</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
       <c r="AC45">
         <v>26</v>
       </c>
@@ -22997,7 +22969,7 @@
         <v>0.96676430476947606</v>
       </c>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J46" t="s">
         <v>55</v>
       </c>
@@ -23062,25 +23034,25 @@
         <v>0.51844804144536372</v>
       </c>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="K47" s="74" t="s">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="K47" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="L47" s="74"/>
-      <c r="M47" s="74"/>
-      <c r="N47" s="74" t="s">
+      <c r="L47" s="73"/>
+      <c r="M47" s="73"/>
+      <c r="N47" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="O47" s="74"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="74" t="s">
+      <c r="O47" s="73"/>
+      <c r="P47" s="73"/>
+      <c r="Q47" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="R47" s="74"/>
-      <c r="S47" s="74" t="s">
+      <c r="R47" s="73"/>
+      <c r="S47" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="T47" s="74"/>
+      <c r="T47" s="73"/>
       <c r="AC47">
         <v>26</v>
       </c>
@@ -23136,7 +23108,7 @@
         <v>4.4061037517890518E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
       <c r="J48" s="53" t="s">
         <v>46</v>
       </c>
@@ -23144,25 +23116,25 @@
         <v>59</v>
       </c>
       <c r="L48" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M48" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M48" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N48" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O48" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P48" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q48" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P48" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q48" s="53" t="s">
+      <c r="R48" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R48" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S48" s="53" t="s">
         <v>51</v>
@@ -23244,7 +23216,7 @@
         <v>7.4781346426718415E-8</v>
       </c>
     </row>
-    <row r="49" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I49" s="53">
         <f>I$9</f>
         <v>34</v>
@@ -23371,7 +23343,7 @@
         <v>3.6079106116507979E-22</v>
       </c>
     </row>
-    <row r="50" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I50" s="53">
         <f>I$10</f>
         <v>27</v>
@@ -23498,7 +23470,7 @@
         <v>4.9700397580905377E-46</v>
       </c>
     </row>
-    <row r="51" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I51" s="53">
         <f>I$11</f>
         <v>26</v>
@@ -23603,7 +23575,7 @@
       <c r="AQ51" s="6"/>
       <c r="AR51" s="6"/>
     </row>
-    <row r="52" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="52" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I52" s="53">
         <f>I$12</f>
         <v>20</v>
@@ -23681,7 +23653,7 @@
       <c r="AQ52" s="6"/>
       <c r="AR52" s="6"/>
     </row>
-    <row r="53" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="53" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I53" s="53">
         <f>I$13</f>
         <v>2</v>
@@ -23780,7 +23752,7 @@
       <c r="AQ53" s="6"/>
       <c r="AR53" s="6"/>
     </row>
-    <row r="54" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="54" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I54" s="53">
         <f>I$14</f>
         <v>13</v>
@@ -23885,7 +23857,7 @@
       <c r="AQ54" s="6"/>
       <c r="AR54" s="6"/>
     </row>
-    <row r="55" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="55" spans="9:47" x14ac:dyDescent="0.25">
       <c r="AC55">
         <v>27</v>
       </c>
@@ -23919,7 +23891,7 @@
       <c r="AQ55" s="6"/>
       <c r="AR55" s="6"/>
     </row>
-    <row r="56" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="56" spans="9:47" x14ac:dyDescent="0.25">
       <c r="J56" t="s">
         <v>55</v>
       </c>
@@ -23962,7 +23934,7 @@
       <c r="AQ56" s="6"/>
       <c r="AR56" s="6"/>
     </row>
-    <row r="57" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="57" spans="9:47" x14ac:dyDescent="0.25">
       <c r="K57" s="53" t="s">
         <v>51</v>
       </c>
@@ -24014,7 +23986,7 @@
       <c r="AQ57" s="6"/>
       <c r="AR57" s="6"/>
     </row>
-    <row r="58" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="58" spans="9:47" x14ac:dyDescent="0.25">
       <c r="J58" s="53" t="s">
         <v>46</v>
       </c>
@@ -24022,25 +23994,25 @@
         <v>59</v>
       </c>
       <c r="L58" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M58" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M58" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N58" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O58" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P58" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q58" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P58" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q58" s="53" t="s">
+      <c r="R58" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R58" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S58" s="53" t="s">
         <v>51</v>
@@ -24099,7 +24071,7 @@
       <c r="AQ58" s="6"/>
       <c r="AR58" s="6"/>
     </row>
-    <row r="59" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="59" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I59" s="53">
         <f>I$9</f>
         <v>34</v>
@@ -24203,7 +24175,7 @@
       <c r="AQ59" s="6"/>
       <c r="AR59" s="6"/>
     </row>
-    <row r="60" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="60" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I60" s="53">
         <f>I$10</f>
         <v>27</v>
@@ -24302,7 +24274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="61" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I61" s="53">
         <f>I$11</f>
         <v>26</v>
@@ -24374,7 +24346,7 @@
         <v>0.99999997459715328</v>
       </c>
     </row>
-    <row r="62" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="62" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I62" s="53">
         <f>I$12</f>
         <v>20</v>
@@ -24467,7 +24439,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="63" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="63" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I63" s="53">
         <f>I$13</f>
         <v>2</v>
@@ -24566,7 +24538,7 @@
         <v>0.98867289643278788</v>
       </c>
     </row>
-    <row r="64" spans="9:47" x14ac:dyDescent="0.3">
+    <row r="64" spans="9:47" x14ac:dyDescent="0.25">
       <c r="I64" s="53">
         <f>I$14</f>
         <v>13</v>
@@ -24665,7 +24637,7 @@
         <v>0.96676430476947606</v>
       </c>
     </row>
-    <row r="65" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="65" spans="9:37" x14ac:dyDescent="0.25">
       <c r="AC65">
         <v>34</v>
       </c>
@@ -24694,7 +24666,7 @@
         <v>0.51844804144536372</v>
       </c>
     </row>
-    <row r="66" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="66" spans="9:37" x14ac:dyDescent="0.25">
       <c r="J66" t="s">
         <v>55</v>
       </c>
@@ -24732,7 +24704,7 @@
         <v>4.4061037517890518E-3</v>
       </c>
     </row>
-    <row r="67" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="67" spans="9:37" x14ac:dyDescent="0.25">
       <c r="K67" s="53" t="s">
         <v>51</v>
       </c>
@@ -24779,7 +24751,7 @@
         <v>7.4781346426718415E-8</v>
       </c>
     </row>
-    <row r="68" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="68" spans="9:37" x14ac:dyDescent="0.25">
       <c r="J68" s="53" t="s">
         <v>46</v>
       </c>
@@ -24787,25 +24759,25 @@
         <v>59</v>
       </c>
       <c r="L68" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M68" s="53" t="s">
         <v>116</v>
-      </c>
-      <c r="M68" s="53" t="s">
-        <v>117</v>
       </c>
       <c r="N68" s="53" t="s">
         <v>58</v>
       </c>
       <c r="O68" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="P68" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q68" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="P68" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q68" s="53" t="s">
+      <c r="R68" s="53" t="s">
         <v>120</v>
-      </c>
-      <c r="R68" s="53" t="s">
-        <v>121</v>
       </c>
       <c r="S68" s="53" t="s">
         <v>51</v>
@@ -24859,7 +24831,7 @@
         <v>3.6079106116507979E-22</v>
       </c>
     </row>
-    <row r="69" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="69" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I69" s="53">
         <f>I$9</f>
         <v>34</v>
@@ -24958,7 +24930,7 @@
         <v>4.9700397580905377E-46</v>
       </c>
     </row>
-    <row r="70" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="70" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I70" s="53">
         <f>I$10</f>
         <v>27</v>
@@ -25031,7 +25003,7 @@
       </c>
       <c r="AC70" s="15"/>
     </row>
-    <row r="71" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="71" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I71" s="53">
         <f>I$11</f>
         <v>26</v>
@@ -25103,7 +25075,7 @@
         <v>0.99999999999719524</v>
       </c>
     </row>
-    <row r="72" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="72" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I72" s="53">
         <f>I$12</f>
         <v>20</v>
@@ -25176,7 +25148,7 @@
       </c>
       <c r="AC72" s="15"/>
     </row>
-    <row r="73" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="73" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I73" s="53">
         <f>I$13</f>
         <v>2</v>
@@ -25249,7 +25221,7 @@
       </c>
       <c r="AC73" s="15"/>
     </row>
-    <row r="74" spans="9:37" x14ac:dyDescent="0.3">
+    <row r="74" spans="9:37" x14ac:dyDescent="0.25">
       <c r="I74" s="53">
         <f>I$14</f>
         <v>13</v>
@@ -25322,11 +25294,19 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="AM9:AU50">
+  <sortState ref="AM9:AU50">
     <sortCondition ref="AM9:AM50"/>
     <sortCondition ref="AN9:AN50"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
     <mergeCell ref="K47:M47"/>
     <mergeCell ref="N47:P47"/>
     <mergeCell ref="Q47:R47"/>
@@ -25339,14 +25319,6 @@
     <mergeCell ref="N37:P37"/>
     <mergeCell ref="Q37:R37"/>
     <mergeCell ref="S37:T37"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:T17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25354,16 +25326,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C17:K69"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>50</v>
       </c>
@@ -25386,7 +25358,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>2</v>
       </c>
@@ -25422,7 +25394,7 @@
         <v>5.3879502695932432E-2</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>2</v>
       </c>
@@ -25458,7 +25430,7 @@
         <v>6.7047460660133145E-4</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>2</v>
       </c>
@@ -25494,7 +25466,7 @@
         <v>6.1569864378397328E-10</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>2</v>
       </c>
@@ -25530,7 +25502,7 @@
         <v>5.0113832165893636E-20</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>2</v>
       </c>
@@ -25566,7 +25538,7 @@
         <v>3.3182053531006217E-40</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>2</v>
       </c>
@@ -25602,7 +25574,7 @@
         <v>9.6325240492643967E-101</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>2</v>
       </c>
@@ -25638,7 +25610,7 @@
         <v>1.2259370561777919E-201</v>
       </c>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>50</v>
       </c>
@@ -25661,7 +25633,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>13</v>
       </c>
@@ -25697,7 +25669,7 @@
         <v>0.33959620249543465</v>
       </c>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>13</v>
       </c>
@@ -25733,7 +25705,7 @@
         <v>6.8334555315952387E-3</v>
       </c>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>13</v>
       </c>
@@ -25769,7 +25741,7 @@
         <v>4.7044436175471894E-9</v>
       </c>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>13</v>
       </c>
@@ -25805,7 +25777,7 @@
         <v>2.4054599814144493E-19</v>
       </c>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>13</v>
       </c>
@@ -25841,7 +25813,7 @@
         <v>6.2880593103970914E-40</v>
       </c>
     </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>13</v>
       </c>
@@ -25877,7 +25849,7 @@
         <v>1.1232388153158255E-101</v>
       </c>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>13</v>
       </c>
@@ -25913,7 +25885,7 @@
         <v>1.3710855645636452E-204</v>
       </c>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>50</v>
       </c>
@@ -25936,7 +25908,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>20</v>
       </c>
@@ -25972,7 +25944,7 @@
         <v>5.8060076427172369E-2</v>
       </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>20</v>
       </c>
@@ -26008,7 +25980,7 @@
         <v>0.52840240070404598</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>20</v>
       </c>
@@ -26044,7 +26016,7 @@
         <v>6.6303089587074629E-4</v>
       </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>20</v>
       </c>
@@ -26080,7 +26052,7 @@
         <v>8.0571842256516554E-10</v>
       </c>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>20</v>
       </c>
@@ -26116,7 +26088,7 @@
         <v>1.1826109965872449E-21</v>
       </c>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>20</v>
       </c>
@@ -26152,7 +26124,7 @@
         <v>3.7394729389817085E-57</v>
       </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>20</v>
       </c>
@@ -26188,7 +26160,7 @@
         <v>2.54736511867457E-116</v>
       </c>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>50</v>
       </c>
@@ -26211,7 +26183,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>26</v>
       </c>
@@ -26247,7 +26219,7 @@
         <v>2.6844268693999487E-2</v>
       </c>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>26</v>
       </c>
@@ -26283,7 +26255,7 @@
         <v>9.3738720526362901E-5</v>
       </c>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>26</v>
       </c>
@@ -26319,7 +26291,7 @@
         <v>2.8047872527050719E-12</v>
       </c>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>26</v>
       </c>
@@ -26355,7 +26327,7 @@
         <v>7.9745353466667782E-25</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>26</v>
       </c>
@@ -26391,7 +26363,7 @@
         <v>6.446302860534334E-50</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>26</v>
       </c>
@@ -26427,7 +26399,7 @@
         <v>3.4050748317249211E-125</v>
       </c>
     </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>26</v>
       </c>
@@ -26463,7 +26435,7 @@
         <v>1.1753122215225618E-250</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E53">
         <v>50</v>
       </c>
@@ -26486,7 +26458,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>27</v>
       </c>
@@ -26522,7 +26494,7 @@
         <v>3.2049182573882548E-2</v>
       </c>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C55">
         <v>27</v>
       </c>
@@ -26558,7 +26530,7 @@
         <v>2.2278564377354874E-5</v>
       </c>
     </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>27</v>
       </c>
@@ -26594,7 +26566,7 @@
         <v>5.9318101389267457E-15</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>27</v>
       </c>
@@ -26630,7 +26602,7 @@
         <v>6.5158927793521139E-31</v>
       </c>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>27</v>
       </c>
@@ -26666,7 +26638,7 @@
         <v>7.8622558119722086E-63</v>
       </c>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>27</v>
       </c>
@@ -26702,7 +26674,7 @@
         <v>1.3812328323043235E-158</v>
       </c>
     </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>27</v>
       </c>
@@ -26738,7 +26710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
       <c r="E62">
         <v>50</v>
       </c>
@@ -26761,7 +26733,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>34</v>
       </c>
@@ -26797,7 +26769,7 @@
         <v>4.1165509565922576E-2</v>
       </c>
     </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>34</v>
       </c>
@@ -26833,7 +26805,7 @@
         <v>0.41239894211341743</v>
       </c>
     </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>34</v>
       </c>
@@ -26869,7 +26841,7 @@
         <v>0.51804100008132037</v>
       </c>
     </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>34</v>
       </c>
@@ -26905,7 +26877,7 @@
         <v>4.4061031186792485E-3</v>
       </c>
     </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>34</v>
       </c>
@@ -26941,7 +26913,7 @@
         <v>7.4781346426716879E-8</v>
       </c>
     </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>34</v>
       </c>
@@ -26977,7 +26949,7 @@
         <v>3.6079106116507979E-22</v>
       </c>
     </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>34</v>
       </c>
@@ -27019,31 +26991,31 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="14" max="14" width="22.5546875" customWidth="1"/>
-    <col min="16" max="16" width="22.5546875" customWidth="1"/>
-    <col min="17" max="17" width="10.109375" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" customWidth="1"/>
-    <col min="20" max="20" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" customWidth="1"/>
     <col min="23" max="23" width="14" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>41</v>
       </c>
@@ -27081,7 +27053,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>3</v>
       </c>
@@ -27122,7 +27094,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
         <v>5</v>
       </c>
@@ -27163,7 +27135,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>6</v>
       </c>
@@ -27204,7 +27176,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>7</v>
       </c>
@@ -27245,7 +27217,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>11</v>
       </c>
@@ -27295,7 +27267,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>12</v>
       </c>
@@ -27359,7 +27331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>13</v>
       </c>
@@ -27413,7 +27385,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>17</v>
       </c>
@@ -27460,7 +27432,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
         <v>19</v>
       </c>
@@ -27514,7 +27486,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>23</v>
       </c>
@@ -27568,7 +27540,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>24</v>
       </c>
@@ -27622,7 +27594,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <v>25</v>
       </c>
@@ -27676,7 +27648,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>26</v>
       </c>
@@ -27730,7 +27702,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="16">
         <v>27</v>
       </c>
@@ -27768,7 +27740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <v>28</v>
       </c>
@@ -27818,7 +27790,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>29</v>
       </c>
@@ -27882,7 +27854,7 @@
         <v>681105.30703300587</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="16">
         <v>30</v>
       </c>
@@ -27945,7 +27917,7 @@
         <v>544072.49190938508</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="16">
         <v>31</v>
       </c>
@@ -27983,7 +27955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>32</v>
       </c>
@@ -28027,7 +27999,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>33</v>
       </c>
@@ -28077,7 +28049,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <v>34</v>
       </c>
@@ -28124,7 +28096,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="16">
         <v>35</v>
       </c>
@@ -28186,7 +28158,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>39</v>
       </c>
@@ -28248,7 +28220,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>43</v>
       </c>
@@ -28286,7 +28258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="17" t="s">
         <v>67</v>
@@ -28301,7 +28273,7 @@
       <c r="J26" s="5"/>
       <c r="L26" s="10"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>2</v>
       </c>
@@ -28342,7 +28314,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>4</v>
       </c>
@@ -28383,7 +28355,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>8</v>
       </c>
@@ -28439,7 +28411,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>10</v>
       </c>
@@ -28495,7 +28467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>18</v>
       </c>
@@ -28551,7 +28523,7 @@
         <v>8.604421011058451E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>38</v>
       </c>
@@ -28607,7 +28579,7 @@
         <v>5.1358836229594522E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>40</v>
       </c>
@@ -28663,7 +28635,7 @@
         <v>5.6786003262642742E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>41</v>
       </c>
@@ -28719,7 +28691,7 @@
         <v>4.936840361445783E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="R35" s="21">
         <v>5</v>
       </c>
@@ -28739,7 +28711,7 @@
         <v>3.3274059405940588E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="R36" s="21">
         <v>6</v>
       </c>

</xml_diff>